<commit_message>
all working including that interactive plot
</commit_message>
<xml_diff>
--- a/general_data/timeline.xlsx
+++ b/general_data/timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20357"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\OneDrive - University College London\Teaching\CASA0005repo\general_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\OneDrive - University College London\Teaching\CASA0005\2020_2021\CASA0005repo\general_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC9815-C0FD-4348-9418-90FA11DEF251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA18495F-86EE-4B89-B212-C91F7E25ED33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6970" xr2:uid="{E1BCC0D3-C0D5-4380-A7FD-21DAAFC42E75}"/>
   </bookViews>
@@ -33,18 +33,12 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>Undertake wider data exploration and reading to find a topic you might be interested in progressing with. I’d recommend starting with a data search first to avoid proposing a research area then forcing potentially unsuitable data to fit it.</t>
-  </si>
-  <si>
     <t>Assess the validity of your topic in terms of data suitability, then sketch out an introduction and literature review including academic and policy documents (or any reputable source).</t>
   </si>
   <si>
     <t>Based on your knowledge of available data and literature compose a research question or hypothesis. Review your introduction and literature review to ensure you are guiding the reader to understanding the importance of the project.</t>
   </si>
   <si>
-    <t>Complete a draft of part 1 of the assignment. The methodology might only be in draft form / initial ideas as we move to more advanced analysis in the second part of the course.</t>
-  </si>
-  <si>
     <t>Learn and practice analysis from the course and identify appropriate techniques (from wider research) that might be applicable/relevant to your data. Conduct an extensive methodological review – this could include analysis from within academic literature and/or government departments (or any reputable source).</t>
   </si>
   <si>
@@ -57,7 +51,13 @@
     <t>Before submission</t>
   </si>
   <si>
-    <t xml:space="preserve">Check that your assignment follows the standard model of scientific investigation. You may need to update part 1 based on the analysis you undertook to ensure a seamless narrative throughout.  </t>
+    <t>Undertake wider data exploration and reading to find a topic you might be interested in progressing with. Start with a data search first to avoid proposing a research area then forcing potentially unsuitable data to fit it.</t>
+  </si>
+  <si>
+    <t>Create a draft of the methodology / initial ideas that can be expanded on as we move to more advanced analysis in the second part of the course.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that your assignment follows the standard model of scientific investigation. You may need to update your introduction and literature review based on the analysis you undertook to ensure a seamless narrative throughout.  </t>
   </si>
 </sst>
 </file>
@@ -119,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -138,6 +138,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EEB7AC-90B9-4FDA-934E-094528D0BE8E}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -476,8 +482,8 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
@@ -485,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" thickBot="1" x14ac:dyDescent="0.9">
@@ -493,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" thickBot="1" x14ac:dyDescent="0.9">
@@ -501,15 +507,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" thickBot="1" x14ac:dyDescent="0.9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
@@ -517,46 +523,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="59.75" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
+      <c r="B8" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="59.75" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>6</v>
+      <c r="B9" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="59.75" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>